<commit_message>
add the def patch to protoanthropology
</commit_message>
<xml_diff>
--- a/src/Wn31_glitches.xlsx
+++ b/src/Wn31_glitches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="600" windowWidth="20175" windowHeight="7425" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="600" windowWidth="20175" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="patches_for_def" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1920" uniqueCount="775">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="780">
   <si>
     <t>patches for wordforms</t>
   </si>
@@ -12103,6 +12103,47 @@
       </rPr>
       <t>} , {enwiki:Osama bin Laden}</t>
     </r>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>daiki.nomura</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>protoanthropology%1:09:00::</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>the study humans prior to the invention of writing</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the study </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> humans prior to the invention of writing</t>
+    </r>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>Simple typo</t>
     <phoneticPr fontId="9"/>
   </si>
   <si>
@@ -12232,7 +12273,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -12266,7 +12307,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="ハイパーリンク" xfId="1" builtinId="8"/>
@@ -12567,8 +12607,8 @@
   </sheetPr>
   <dimension ref="A1:C469"/>
   <sheetViews>
-    <sheetView topLeftCell="A446" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A465" sqref="A465"/>
+    <sheetView tabSelected="1" topLeftCell="A448" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B470" sqref="B470"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -15673,22 +15713,44 @@
       <c r="B464" s="21"/>
     </row>
     <row r="465" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A465" s="23"/>
-      <c r="B465" s="9"/>
+      <c r="A465" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B465" s="9" t="s">
+        <v>775</v>
+      </c>
     </row>
     <row r="466" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A466" s="18"/>
-      <c r="B466" s="9"/>
+      <c r="A466" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B466" s="9" t="s">
+        <v>776</v>
+      </c>
     </row>
     <row r="467" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A467" s="18"/>
+      <c r="A467" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B467" s="9" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="468" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A468" s="19"/>
+      <c r="A468" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="B468" s="9" t="s">
+        <v>778</v>
+      </c>
     </row>
     <row r="469" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A469" s="18"/>
-      <c r="B469" s="9"/>
+      <c r="A469" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B469" s="9" t="s">
+        <v>779</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="9"/>
@@ -15701,7 +15763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A512" workbookViewId="0">
+    <sheetView topLeftCell="A512" workbookViewId="0">
       <selection activeCell="A523" sqref="A523"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updateted README.md a liitle
For a detailed comment, this should work probably but I am not sure
whether it really works...
</commit_message>
<xml_diff>
--- a/src/Wn31_glitches.xlsx
+++ b/src/Wn31_glitches.xlsx
@@ -12118,10 +12118,6 @@
     <phoneticPr fontId="9"/>
   </si>
   <si>
-    <t>daiki.nomura</t>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
     <t>keep_track%2:31:00::</t>
     <phoneticPr fontId="9"/>
   </si>
@@ -12359,10 +12355,6 @@
     <phoneticPr fontId="9"/>
   </si>
   <si>
-    <t xml:space="preserve">{enwiki:Immigration and Naturalization Service} INS was splitted into three and transferred from the Department of Justice to Department of Homeland Security. The holonym of this synset refers to Department of Homeland Security and at the sametime, def refers to Department of Justice. This is inconsistancy and I think adding "former" could be the minimal way to solve this. There are many troubles in the hyponyms of "Department". </t>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
     <t>house_painter%1:18:00::</t>
     <phoneticPr fontId="9"/>
   </si>
@@ -12400,7 +12392,15 @@
     <phoneticPr fontId="9"/>
   </si>
   <si>
-    <t>daiki.nomura</t>
+    <t>daiki.nomura, EW_PULLED</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>daiki.nomura, EW_PULL...</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>{enwiki:Immigration and Naturalization Service} INS was transferred from the Department of Justice to Department of Homeland Security(2003). The holonym of this synset is already Department of Homeland Security but def says it is in the Department of Justice. This is inconsistancy and I think adding "former" could be the minimal way to solve this.</t>
     <phoneticPr fontId="9"/>
   </si>
 </sst>
@@ -12868,8 +12868,8 @@
   </sheetPr>
   <dimension ref="A1:C505"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A486" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A506" sqref="A506"/>
+    <sheetView tabSelected="1" topLeftCell="A484" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B500" sqref="B500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -14107,7 +14107,7 @@
         <v>25</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="15.75" customHeight="1">
@@ -14115,7 +14115,7 @@
         <v>111</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="187" spans="1:2" ht="15.75" customHeight="1">
@@ -14123,7 +14123,7 @@
         <v>10</v>
       </c>
       <c r="B187" s="9" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="189" spans="1:2" ht="15.75" customHeight="1">
@@ -14163,7 +14163,7 @@
         <v>10</v>
       </c>
       <c r="B193" s="9" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="195" spans="1:3" ht="15.75" customHeight="1">
@@ -16010,7 +16010,7 @@
         <v>10</v>
       </c>
       <c r="B469" s="9" t="s">
-        <v>777</v>
+        <v>806</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="15.75" customHeight="1">
@@ -16018,7 +16018,7 @@
         <v>1</v>
       </c>
       <c r="B471" s="10" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="472" spans="1:2" ht="15.75" customHeight="1">
@@ -16026,7 +16026,7 @@
         <v>16</v>
       </c>
       <c r="B472" s="9" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="473" spans="1:2" ht="15.75" customHeight="1">
@@ -16034,7 +16034,7 @@
         <v>25</v>
       </c>
       <c r="B473" s="9" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="474" spans="1:2" ht="15.75" customHeight="1">
@@ -16042,7 +16042,7 @@
         <v>111</v>
       </c>
       <c r="B474" s="9" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="475" spans="1:2" ht="15.75" customHeight="1">
@@ -16050,7 +16050,7 @@
         <v>10</v>
       </c>
       <c r="B475" s="9" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="477" spans="1:2" ht="15.75" customHeight="1">
@@ -16058,7 +16058,7 @@
         <v>1</v>
       </c>
       <c r="B477" s="10" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="478" spans="1:2" ht="15.75" customHeight="1">
@@ -16066,7 +16066,7 @@
         <v>16</v>
       </c>
       <c r="B478" s="9" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="479" spans="1:2" ht="15.75" customHeight="1">
@@ -16074,7 +16074,7 @@
         <v>25</v>
       </c>
       <c r="B479" s="9" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="480" spans="1:2" ht="15.75" customHeight="1">
@@ -16082,7 +16082,7 @@
         <v>111</v>
       </c>
       <c r="B480" s="9" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="481" spans="1:2" ht="15.75" customHeight="1">
@@ -16090,7 +16090,7 @@
         <v>10</v>
       </c>
       <c r="B481" s="9" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="483" spans="1:2" ht="15.75" customHeight="1">
@@ -16098,7 +16098,7 @@
         <v>1</v>
       </c>
       <c r="B483" s="9" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="484" spans="1:2" ht="15.75" customHeight="1">
@@ -16106,7 +16106,7 @@
         <v>16</v>
       </c>
       <c r="B484" s="9" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="485" spans="1:2" ht="15.75" customHeight="1">
@@ -16114,7 +16114,7 @@
         <v>25</v>
       </c>
       <c r="B485" s="9" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="486" spans="1:2" ht="15.75" customHeight="1">
@@ -16122,7 +16122,7 @@
         <v>111</v>
       </c>
       <c r="B486" s="9" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="487" spans="1:2" ht="15.75" customHeight="1">
@@ -16130,7 +16130,7 @@
         <v>10</v>
       </c>
       <c r="B487" s="9" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="489" spans="1:2" ht="15.75" customHeight="1">
@@ -16138,7 +16138,7 @@
         <v>1</v>
       </c>
       <c r="B489" s="10" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="490" spans="1:2" ht="15.75" customHeight="1">
@@ -16146,7 +16146,7 @@
         <v>16</v>
       </c>
       <c r="B490" s="9" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="491" spans="1:2" ht="15.75" customHeight="1">
@@ -16154,7 +16154,7 @@
         <v>25</v>
       </c>
       <c r="B491" s="9" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="492" spans="1:2" ht="15.75" customHeight="1">
@@ -16162,7 +16162,7 @@
         <v>111</v>
       </c>
       <c r="B492" s="9" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="493" spans="1:2" ht="15.75" customHeight="1">
@@ -16170,7 +16170,7 @@
         <v>10</v>
       </c>
       <c r="B493" s="9" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="495" spans="1:2" ht="15.75" customHeight="1">
@@ -16178,7 +16178,7 @@
         <v>1</v>
       </c>
       <c r="B495" s="9" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="496" spans="1:2" ht="15.75" customHeight="1">
@@ -16186,7 +16186,7 @@
         <v>16</v>
       </c>
       <c r="B496" s="9" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="497" spans="1:2" ht="15.75" customHeight="1">
@@ -16194,15 +16194,15 @@
         <v>25</v>
       </c>
       <c r="B497" s="9" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="498" spans="1:2" ht="40.5" customHeight="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="498" spans="1:2" ht="28.5" customHeight="1">
       <c r="A498" s="19" t="s">
         <v>111</v>
       </c>
       <c r="B498" s="10" t="s">
-        <v>803</v>
+        <v>808</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="15.75" customHeight="1">
@@ -16210,7 +16210,7 @@
         <v>10</v>
       </c>
       <c r="B499" s="9" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="15.75" customHeight="1">
@@ -16218,7 +16218,7 @@
         <v>1</v>
       </c>
       <c r="B501" s="9" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="15.75" customHeight="1">
@@ -16226,7 +16226,7 @@
         <v>16</v>
       </c>
       <c r="B502" s="9" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="15.75" customHeight="1">
@@ -16234,7 +16234,7 @@
         <v>25</v>
       </c>
       <c r="B503" s="9" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="15.75" customHeight="1">
@@ -16242,7 +16242,7 @@
         <v>111</v>
       </c>
       <c r="B504" s="9" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="15.75" customHeight="1">
@@ -16250,7 +16250,7 @@
         <v>10</v>
       </c>
       <c r="B505" s="9" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed an article error in the commment of INS.
</commit_message>
<xml_diff>
--- a/src/Wn31_glitches.xlsx
+++ b/src/Wn31_glitches.xlsx
@@ -12326,8 +12326,61 @@
     <phoneticPr fontId="9"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">an </t>
+    <t>daiki.nomura</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>house_painter%1:18:00::</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>a painter of houses a similar buildings</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a painter of houses </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> similar buildings</t>
+    </r>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>Simple typo</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>daiki.nomura, EW_PULLED</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>daiki.nomura, EW_PULL...</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>{enwiki:Immigration and Naturalization Service} INS was transferred from the Department of Justice to Department of Homeland Security(2003). The holonym of this synset is already Department of Homeland Security but def says it is in the Department of Justice. This is inconsistancy and I think adding "former" could be the minimal way to solve this.</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">a </t>
     </r>
     <r>
       <rPr>
@@ -12348,59 +12401,6 @@
       </rPr>
       <t xml:space="preserve"> agency in the Department of Justice that enforces laws and regulations for the admission of foreign-born persons to the United States</t>
     </r>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
-    <t>daiki.nomura</t>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
-    <t>house_painter%1:18:00::</t>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
-    <t>a painter of houses a similar buildings</t>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">a painter of houses </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>or</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> similar buildings</t>
-    </r>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
-    <t>Simple typo</t>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
-    <t>daiki.nomura, EW_PULLED</t>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
-    <t>daiki.nomura, EW_PULL...</t>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
-    <t>{enwiki:Immigration and Naturalization Service} INS was transferred from the Department of Justice to Department of Homeland Security(2003). The holonym of this synset is already Department of Homeland Security but def says it is in the Department of Justice. This is inconsistancy and I think adding "former" could be the minimal way to solve this.</t>
     <phoneticPr fontId="9"/>
   </si>
 </sst>
@@ -12869,7 +12869,7 @@
   <dimension ref="A1:C505"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A484" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B500" sqref="B500"/>
+      <selection activeCell="B499" sqref="B499"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -16010,7 +16010,7 @@
         <v>10</v>
       </c>
       <c r="B469" s="9" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="471" spans="1:2" ht="15.75" customHeight="1">
@@ -16194,7 +16194,7 @@
         <v>25</v>
       </c>
       <c r="B497" s="9" t="s">
-        <v>800</v>
+        <v>808</v>
       </c>
     </row>
     <row r="498" spans="1:2" ht="28.5" customHeight="1">
@@ -16202,7 +16202,7 @@
         <v>111</v>
       </c>
       <c r="B498" s="10" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="499" spans="1:2" ht="15.75" customHeight="1">
@@ -16210,7 +16210,7 @@
         <v>10</v>
       </c>
       <c r="B499" s="9" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="501" spans="1:2" ht="15.75" customHeight="1">
@@ -16218,7 +16218,7 @@
         <v>1</v>
       </c>
       <c r="B501" s="9" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="502" spans="1:2" ht="15.75" customHeight="1">
@@ -16226,7 +16226,7 @@
         <v>16</v>
       </c>
       <c r="B502" s="9" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="503" spans="1:2" ht="15.75" customHeight="1">
@@ -16234,7 +16234,7 @@
         <v>25</v>
       </c>
       <c r="B503" s="9" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="504" spans="1:2" ht="15.75" customHeight="1">
@@ -16242,7 +16242,7 @@
         <v>111</v>
       </c>
       <c r="B504" s="9" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="505" spans="1:2" ht="15.75" customHeight="1">
@@ -16250,7 +16250,7 @@
         <v>10</v>
       </c>
       <c r="B505" s="9" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 1 preposition lack fix and 1 year fix.
</commit_message>
<xml_diff>
--- a/src/Wn31_glitches.xlsx
+++ b/src/Wn31_glitches.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2286" uniqueCount="913">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2306" uniqueCount="923">
   <si>
     <t>patches for wordforms</t>
   </si>
@@ -14053,6 +14053,120 @@
       </rPr>
       <t xml:space="preserve"> from one species to another species</t>
     </r>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>breviary%1:10:00::</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>aiki.nomura</t>
+    </r>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>(Roman Catholic Church) a book of prayers to be recited daily certain priests and members of religious orders</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>Simple typo.</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(Roman Catholic Church) a book of prayers to be recited daily </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>by</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> certain priests and members of religious orders</t>
+    </r>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>Augsburg_Confession%1:10:00::</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the document drawn up in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1555</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to defend the catholicity of Lutheran doctrine and to justify innovations in Lutheran practice; is still in effect today</t>
+    </r>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the document drawn up in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1530</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> to defend the catholicity of Lutheran doctrine and to justify innovations in Lutheran practice; is still in effect today</t>
+    </r>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>daiki.nomura</t>
+    <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>The Augsburg Confession has been compiled by German Protestant princes in 1530. Probably there are confusion between Augsburg Confession(1530) and Peace of Augsburg(1555). ... {enwiki:Augsburg Confession},{enwiki:Peace of Augsburg}</t>
     <phoneticPr fontId="9"/>
   </si>
 </sst>
@@ -14521,10 +14635,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C673"/>
+  <dimension ref="A1:C685"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A651" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A674" sqref="A674"/>
+    <sheetView tabSelected="1" topLeftCell="A667" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A686" sqref="A686"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -19026,6 +19140,86 @@
       </c>
       <c r="B673" s="9" t="s">
         <v>891</v>
+      </c>
+    </row>
+    <row r="675" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A675" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B675" s="9" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="676" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A676" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B676" s="9" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="677" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A677" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B677" s="9" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="678" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A678" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B678" s="9" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="679" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A679" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B679" s="9" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="681" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A681" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="B681" s="9" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="682" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A682" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B682" s="9" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="683" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A683" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B683" s="9" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="684" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A684" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="B684" s="9" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="685" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A685" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B685" s="9" t="s">
+        <v>921</v>
       </c>
     </row>
   </sheetData>

</xml_diff>